<commit_message>
Added kimppakohde to tests
</commit_message>
<xml_diff>
--- a/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
+++ b/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t xml:space="preserve">UrakoitsijaId</t>
   </si>
@@ -210,6 +210,39 @@
   </si>
   <si>
     <t xml:space="preserve">15.2.2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-0000123-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">134567890B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIRKKOÄYRÄÄNTIE 1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16200 ARTJÄRVI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOHN LINDROTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660 L ENERGIAJÄTEASTIA TYHJENNYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-0000999-99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIRKKOÄYRÄÄN ENERGIAKIMPPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-1110999-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KIRKKOÄYRÄÄNTIE 11</t>
   </si>
 </sst>
 </file>
@@ -220,7 +253,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,6 +274,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -285,7 +323,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -295,6 +333,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -315,53 +357,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AR3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="42.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="45.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -370,103 +418,103 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="0" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="0" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="0" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="0" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="0" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="0" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="0" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="0" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="0" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="0" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="0" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="0" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="0" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -486,80 +534,169 @@
       <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>49</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="M2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="Q2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="S2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB2" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="AC2" s="0" t="s">
+      <c r="AC2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="0" t="s">
+      <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AP2" s="0" t="n">
+      <c r="AP2" s="1" t="n">
         <v>398</v>
       </c>
-      <c r="AQ2" s="0" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AR2" s="0" t="s">
+      <c r="AR2" s="1" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a kimppa partner to test data
</commit_message>
<xml_diff>
--- a/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
+++ b/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t xml:space="preserve">UrakoitsijaId</t>
   </si>
@@ -246,6 +246,21 @@
   </si>
   <si>
     <t xml:space="preserve">KIRKKOÄYRÄÄNTIE 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-0000123-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100456789B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KUVAKALLIONTIE 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15230 LAHTI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIKU FORSSTRÖM</t>
   </si>
 </sst>
 </file>
@@ -326,7 +341,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -336,6 +351,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,10 +379,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -372,19 +391,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="42.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="22.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="45.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="33.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="17.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="23.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="33.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="17.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="23.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +660,7 @@
       <c r="N3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>53</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -650,31 +669,31 @@
       <c r="R3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>69</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>53</v>
       </c>
       <c r="AC3" s="1" t="s">
@@ -683,22 +702,111 @@
       <c r="AD3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN3" s="0" t="s">
+      <c r="AN3" s="1" t="s">
         <v>74</v>
       </c>
       <c r="AO3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AP3" s="0" t="n">
+      <c r="AP3" s="1" t="n">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP4" s="1" t="n">
         <v>560</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Setting osapuolenroolit for each jätetyyppi, also tests included. Doesn't create all roles to kohde.
</commit_message>
<xml_diff>
--- a/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
+++ b/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="89">
   <si>
     <t xml:space="preserve">UrakoitsijaId</t>
   </si>
@@ -179,7 +179,7 @@
     <t xml:space="preserve">HEIKKI LEHMUSTO</t>
   </si>
   <si>
-    <t xml:space="preserve">VESIJÃ„RVENKATU 8</t>
+    <t xml:space="preserve">VESIJÄRVENKATU 8</t>
   </si>
   <si>
     <t xml:space="preserve">FI</t>
@@ -194,7 +194,7 @@
     <t xml:space="preserve">Sekaj</t>
   </si>
   <si>
-    <t xml:space="preserve">660 L SEKAJÃ„TEASTIA TYHJENNYS</t>
+    <t xml:space="preserve">660 L SEKAJÄTEASTIA TYHJENNYS</t>
   </si>
   <si>
     <t xml:space="preserve">0,66</t>
@@ -212,6 +212,39 @@
     <t xml:space="preserve">15.2.2023</t>
   </si>
   <si>
+    <t xml:space="preserve">Lasi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 L LASIJÄTEASTIA TYHJENNYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metalli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 L METALLIASTIA TYHJENNYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kartonki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660 L KARTONKIASTIA TYHJENNYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muovi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">660 L PAKKAUSMUOVIASTIA TYHJENNYS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 L BIOJÄTEASTIA TYHJENNYS</t>
+  </si>
+  <si>
     <t xml:space="preserve">01-0000123-01</t>
   </si>
   <si>
@@ -230,16 +263,10 @@
     <t xml:space="preserve">JOHN LINDROTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Energia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">660 L ENERGIAJÄTEASTIA TYHJENNYS</t>
-  </si>
-  <si>
     <t xml:space="preserve">01-0000999-99</t>
   </si>
   <si>
-    <t xml:space="preserve">KIRKKOÄYRÄÄN ENERGIAKIMPPA</t>
+    <t xml:space="preserve">KIRKKOÄYRÄÄN SEKAKIMPPA</t>
   </si>
   <si>
     <t xml:space="preserve">01-1110999-01</t>
@@ -271,7 +298,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -292,11 +319,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -354,11 +376,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,10 +401,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,29 +658,38 @@
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B3" s="1" t="n">
+        <v>6761402</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>427353</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>53</v>
@@ -670,26 +701,27 @@
         <v>55</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="U3" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="X3" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="Y3" s="1" t="n">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="Z3" s="1"/>
       <c r="AA3" s="1" t="n">
         <v>1</v>
       </c>
@@ -702,54 +734,50 @@
       <c r="AD3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AM3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="AP3" s="1" t="n">
-        <v>560</v>
-      </c>
+        <v>398</v>
+      </c>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="B4" s="1" t="n">
+        <v>6761402</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>427353</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>76</v>
+        <v>46</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>79</v>
+        <v>49</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="O4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>53</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -759,30 +787,31 @@
         <v>55</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="U4" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="V4" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="U4" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="V4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X4" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="Y4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="1" t="n">
         <v>53</v>
       </c>
       <c r="AC4" s="1" t="s">
@@ -791,28 +820,453 @@
       <c r="AD4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AK4" s="1" t="s">
+      <c r="AP4" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>6761402</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>427353</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP5" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>6761402</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>427353</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="AL4" s="1" t="s">
+      <c r="U6" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP6" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6761402</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>427353</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AM4" s="1" t="s">
+      <c r="T7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="AN4" s="1" t="s">
+      <c r="U7" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AP7" s="1" t="n">
+        <v>398</v>
+      </c>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AO4" s="1" t="s">
+      <c r="F8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U8" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="AP4" s="1" t="n">
+      <c r="V8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP8" s="1" t="n">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U9" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="X9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AN9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AO9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP9" s="1" t="n">
         <v>560</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Käytä aiemmin määritettyä asiakkuutta." errorStyle="stop" errorTitle="Asiakas jo olemassa" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J1001" type="custom">
+    <dataValidation allowBlank="true" error="Käytä aiemmin määritettyä asiakkuutta." errorStyle="stop" errorTitle="Asiakas jo olemassa" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J1006" type="custom">
       <formula1>OR(#ref!="",COUNTIF(#ref!,#ref!)&lt;2)</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Fixed ids in test data
</commit_message>
<xml_diff>
--- a/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
+++ b/tests/data/test_lahti_siirtotiedosto/kuljetustiedot_excel.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="88">
   <si>
     <t xml:space="preserve">UrakoitsijaId</t>
   </si>
@@ -267,9 +267,6 @@
   </si>
   <si>
     <t xml:space="preserve">KIRKKOÄYRÄÄN SEKAKIMPPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01-1110999-01</t>
   </si>
   <si>
     <t xml:space="preserve">KIRKKOÄYRÄÄNTIE 11</t>
@@ -376,7 +373,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,8 +400,8 @@
   </sheetPr>
   <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AF1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AL8" activeCellId="0" sqref="AL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1163,10 +1160,10 @@
         <v>81</v>
       </c>
       <c r="AM8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN8" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AN8" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AO8" s="1" t="s">
         <v>77</v>
@@ -1180,28 +1177,28 @@
         <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>53</v>
@@ -1252,10 +1249,10 @@
         <v>81</v>
       </c>
       <c r="AM9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN9" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="AN9" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="AO9" s="1" t="s">
         <v>77</v>

</xml_diff>